<commit_message>
update do product backlog
</commit_message>
<xml_diff>
--- a/Documentacao/Documentacao/ProductBacklog.xlsx
+++ b/Documentacao/Documentacao/ProductBacklog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projeto de PI\Project2nd\Documentacao\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C44D9-05D1-4705-AD25-7CF76A969A3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -267,12 +266,36 @@
   </si>
   <si>
     <t>RNF012</t>
+  </si>
+  <si>
+    <t>Aplicação JAVA</t>
+  </si>
+  <si>
+    <t>Aplicação para desktop listando processos</t>
+  </si>
+  <si>
+    <t>RF018</t>
+  </si>
+  <si>
+    <t>RF019</t>
+  </si>
+  <si>
+    <t>RF020</t>
+  </si>
+  <si>
+    <t>Tela de login em swing</t>
+  </si>
+  <si>
+    <t>Exibir dados de CPU, memória, disco, RAM com OSHI</t>
+  </si>
+  <si>
+    <t>Listar os processos que estão em execução com OSHI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,31 +639,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,6 +669,56 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,11 +1039,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1111,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="62">
+      <c r="A5" s="54">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1076,7 +1125,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62">
+      <c r="A6" s="54">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1090,7 +1139,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
+      <c r="A7" s="54">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1103,18 +1152,31 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="73">
+        <v>7</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="75">
+        <v>5</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,13 +1208,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
+      <c r="A2" s="65">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="56" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="11">
@@ -1164,25 +1226,25 @@
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="56" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="11">
         <v>3</v>
       </c>
-      <c r="E3" s="65"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="58" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="43">
@@ -1192,11 +1254,11 @@
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="58" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="43">
@@ -1206,14 +1268,14 @@
         <v>2</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="67"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="56" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="11">
@@ -1223,14 +1285,14 @@
         <v>3</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="69"/>
+      <c r="G6" s="61"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="56" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="11">
@@ -1240,11 +1302,11 @@
         <v>5</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="68"/>
+      <c r="G7" s="60"/>
       <c r="J7" s="42"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="15" t="s">
         <v>22</v>
       </c>
@@ -1260,16 +1322,16 @@
       <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="50">
+      <c r="A9" s="68">
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="62">
         <v>3</v>
       </c>
       <c r="E9" s="12">
@@ -1280,14 +1342,14 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="71">
+      <c r="D10" s="63">
         <v>3</v>
       </c>
       <c r="E10" s="36">
@@ -1296,11 +1358,11 @@
       <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="58" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="43">
@@ -1312,14 +1374,14 @@
       <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="57">
         <v>3</v>
       </c>
       <c r="E12" s="11">
@@ -1328,16 +1390,16 @@
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="53">
+      <c r="A13" s="71">
         <v>3</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="57">
         <v>5</v>
       </c>
       <c r="E13" s="11">
@@ -1346,11 +1408,11 @@
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="56" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="11">
@@ -1368,24 +1430,24 @@
       <c r="B15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="58" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="21">
         <v>4</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="70">
+      <c r="D16" s="62">
         <v>4</v>
       </c>
       <c r="E16" s="28"/>
@@ -1405,14 +1467,62 @@
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="20"/>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="79">
+        <v>7</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="82">
+        <v>4</v>
+      </c>
+      <c r="E18" s="64"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="82">
+        <v>4</v>
+      </c>
+      <c r="E19" s="83"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="80"/>
+      <c r="B20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="78">
+        <v>4</v>
+      </c>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1420,11 +1530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1566,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
+      <c r="A2" s="65">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -1471,24 +1581,24 @@
       <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="57"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="54" t="s">
+      <c r="A3" s="67"/>
+      <c r="B3" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="24">
         <v>4</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="57"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="48">
+      <c r="A4" s="66">
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
@@ -1504,7 +1614,7 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="14" t="s">
         <v>51</v>
       </c>
@@ -1514,7 +1624,7 @@
       <c r="D5" s="12">
         <v>5</v>
       </c>
-      <c r="E5" s="56"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="10" t="s">
         <v>56</v>
       </c>
@@ -1532,11 +1642,11 @@
       <c r="D6" s="35">
         <v>4</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="A7" s="65">
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1548,11 +1658,11 @@
       <c r="D7" s="12">
         <v>5</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="16" t="s">
         <v>54</v>
       </c>
@@ -1562,11 +1672,11 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="58"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="16" t="s">
         <v>77</v>
       </c>
@@ -1576,11 +1686,11 @@
       <c r="D9" s="12">
         <v>3</v>
       </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="16" t="s">
         <v>29</v>
       </c>
@@ -1590,11 +1700,11 @@
       <c r="D10" s="12">
         <v>3</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="58"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="15" t="s">
         <v>57</v>
       </c>
@@ -1608,10 +1718,10 @@
         <v>2</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="J11" s="61"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="65">
         <v>6</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -1627,7 +1737,7 @@
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="15" t="s">
         <v>79</v>
       </c>

</xml_diff>